<commit_message>
7 de junho - casa
</commit_message>
<xml_diff>
--- a/mieec-distrib-v2014/outras_cenas/referencias.xlsx
+++ b/mieec-distrib-v2014/outras_cenas/referencias.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17726"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marisa\Master-Thesis\mieec-distrib-v2014\outras_cenas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marisa Oliveira\Documents\GitHub\Master-Thesis\mieec-distrib-v2014\outras_cenas\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="93">
   <si>
     <t>REF</t>
   </si>
@@ -291,6 +291,18 @@
   </si>
   <si>
     <t>I/O Design Flexibility with the FPGA Mezzanine Card (FMC)</t>
+  </si>
+  <si>
+    <t>R031</t>
+  </si>
+  <si>
+    <t>XAPP</t>
+  </si>
+  <si>
+    <t>sim</t>
+  </si>
+  <si>
+    <t>Implementing SMPTE SDI Interfaces with 7 Series Transceivers</t>
   </si>
 </sst>
 </file>
@@ -319,7 +331,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -346,6 +358,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -398,11 +416,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -415,15 +430,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -434,6 +440,21 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -717,901 +738,953 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N33"/>
+  <dimension ref="A1:N34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="E34" sqref="E34:L34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2"/>
-    <col min="2" max="2" width="13.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="14.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="11" width="9.140625" style="2"/>
-    <col min="12" max="12" width="40.85546875" style="2" customWidth="1"/>
-    <col min="13" max="13" width="9.140625" style="2"/>
-    <col min="14" max="14" width="10.85546875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="11" width="9.140625" style="1"/>
+    <col min="12" max="12" width="40.85546875" style="1" customWidth="1"/>
+    <col min="13" max="13" width="9.140625" style="1"/>
+    <col min="14" max="14" width="10.85546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
+      <c r="K2" s="10"/>
+      <c r="L2" s="10"/>
+      <c r="M2" s="10"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="4" t="s">
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11"/>
+      <c r="M3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="N3" s="3" t="s">
+      <c r="N3" s="2" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
-      <c r="J4" s="7"/>
-      <c r="K4" s="7"/>
-      <c r="L4" s="7"/>
-      <c r="M4" s="12" t="s">
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="12"/>
+      <c r="K4" s="12"/>
+      <c r="L4" s="12"/>
+      <c r="M4" s="8" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="8"/>
-      <c r="J5" s="8"/>
-      <c r="K5" s="8"/>
-      <c r="L5" s="8"/>
-      <c r="M5" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="N5" s="2">
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9"/>
+      <c r="M5" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="N5" s="1">
         <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="E6" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
-      <c r="J6" s="8"/>
-      <c r="K6" s="8"/>
-      <c r="L6" s="8"/>
-      <c r="M6" s="9" t="s">
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="9"/>
+      <c r="M6" s="5" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="E7" s="8" t="s">
+      <c r="E7" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="8"/>
-      <c r="K7" s="8"/>
-      <c r="L7" s="8"/>
-      <c r="M7" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="N7" s="2">
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="9"/>
+      <c r="M7" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="N7" s="1">
         <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E8" s="8" t="s">
+      <c r="E8" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="8"/>
-      <c r="J8" s="8"/>
-      <c r="K8" s="8"/>
-      <c r="L8" s="8"/>
-      <c r="M8" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="N8" s="2">
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="N8" s="1">
         <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E9" s="8" t="s">
+      <c r="E9" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8"/>
-      <c r="K9" s="8"/>
-      <c r="L9" s="8"/>
-      <c r="M9" s="9" t="s">
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="9"/>
+      <c r="M9" s="5" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10" s="1">
         <v>2014</v>
       </c>
-      <c r="E10" s="8" t="s">
+      <c r="E10" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="8"/>
-      <c r="J10" s="8"/>
-      <c r="K10" s="8"/>
-      <c r="L10" s="8"/>
-      <c r="M10" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="N10" s="2">
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="9"/>
+      <c r="L10" s="9"/>
+      <c r="M10" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="N10" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11" s="1">
         <v>2014</v>
       </c>
-      <c r="E11" s="8" t="s">
+      <c r="E11" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
-      <c r="I11" s="8"/>
-      <c r="J11" s="8"/>
-      <c r="K11" s="8"/>
-      <c r="L11" s="8"/>
-      <c r="M11" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="N11" s="2">
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="9"/>
+      <c r="K11" s="9"/>
+      <c r="L11" s="9"/>
+      <c r="M11" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="N11" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D12" s="1">
         <v>2014</v>
       </c>
-      <c r="E12" s="8" t="s">
+      <c r="E12" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="8"/>
-      <c r="J12" s="8"/>
-      <c r="K12" s="8"/>
-      <c r="L12" s="8"/>
-      <c r="M12" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="N12" s="2">
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="9"/>
+      <c r="K12" s="9"/>
+      <c r="L12" s="9"/>
+      <c r="M12" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="N12" s="1">
         <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D13" s="2">
+      <c r="D13" s="1">
         <v>2013</v>
       </c>
-      <c r="E13" s="8" t="s">
+      <c r="E13" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
-      <c r="I13" s="8"/>
-      <c r="J13" s="8"/>
-      <c r="K13" s="8"/>
-      <c r="L13" s="8"/>
-      <c r="M13" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="N13" s="2">
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9"/>
+      <c r="K13" s="9"/>
+      <c r="L13" s="9"/>
+      <c r="M13" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="N13" s="1">
         <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="D14" s="2">
+      <c r="D14" s="1">
         <v>2016</v>
       </c>
-      <c r="E14" s="8" t="s">
+      <c r="E14" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="8"/>
-      <c r="I14" s="8"/>
-      <c r="J14" s="8"/>
-      <c r="K14" s="8"/>
-      <c r="L14" s="8"/>
-      <c r="M14" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="N14" s="2">
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="9"/>
+      <c r="K14" s="9"/>
+      <c r="L14" s="9"/>
+      <c r="M14" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="N14" s="1">
         <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D15" s="11" t="s">
+      <c r="D15" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="E15" s="8" t="s">
+      <c r="E15" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="8"/>
-      <c r="I15" s="8"/>
-      <c r="J15" s="8"/>
-      <c r="K15" s="8"/>
-      <c r="L15" s="8"/>
-      <c r="M15" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="N15" s="2">
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="9"/>
+      <c r="K15" s="9"/>
+      <c r="L15" s="9"/>
+      <c r="M15" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="N15" s="1">
         <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D16" s="2">
+      <c r="D16" s="1">
         <v>2015</v>
       </c>
-      <c r="E16" s="8" t="s">
+      <c r="E16" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="8"/>
-      <c r="I16" s="8"/>
-      <c r="J16" s="8"/>
-      <c r="K16" s="8"/>
-      <c r="L16" s="8"/>
-      <c r="M16" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="N16" s="2">
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="9"/>
+      <c r="K16" s="9"/>
+      <c r="L16" s="9"/>
+      <c r="M16" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="N16" s="1">
         <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C17" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D17" s="2">
+      <c r="D17" s="1">
         <v>2014</v>
       </c>
-      <c r="E17" s="8" t="s">
+      <c r="E17" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="8"/>
-      <c r="I17" s="8"/>
-      <c r="J17" s="8"/>
-      <c r="K17" s="8"/>
-      <c r="L17" s="8"/>
-      <c r="M17" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="N17" s="2">
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="9"/>
+      <c r="K17" s="9"/>
+      <c r="L17" s="9"/>
+      <c r="M17" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="N17" s="1">
         <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="D18" s="2">
+      <c r="D18" s="1">
         <v>2016</v>
       </c>
-      <c r="E18" s="8" t="s">
+      <c r="E18" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="8"/>
-      <c r="I18" s="8"/>
-      <c r="J18" s="8"/>
-      <c r="K18" s="8"/>
-      <c r="L18" s="8"/>
-      <c r="M18" s="9" t="s">
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="9"/>
+      <c r="K18" s="9"/>
+      <c r="L18" s="9"/>
+      <c r="M18" s="5" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C19" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D19" s="11" t="s">
+      <c r="D19" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="E19" s="8" t="s">
+      <c r="E19" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="8"/>
-      <c r="I19" s="8"/>
-      <c r="J19" s="8"/>
-      <c r="K19" s="8"/>
-      <c r="L19" s="8"/>
-      <c r="M19" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="N19" s="2">
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="9"/>
+      <c r="L19" s="9"/>
+      <c r="M19" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="N19" s="1">
         <v>6</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C20" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D20" s="2">
+      <c r="D20" s="1">
         <v>2012</v>
       </c>
-      <c r="E20" s="8" t="s">
+      <c r="E20" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="F20" s="8"/>
-      <c r="G20" s="8"/>
-      <c r="H20" s="8"/>
-      <c r="I20" s="8"/>
-      <c r="J20" s="8"/>
-      <c r="K20" s="8"/>
-      <c r="L20" s="8"/>
-      <c r="M20" s="9" t="s">
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="9"/>
+      <c r="K20" s="9"/>
+      <c r="L20" s="9"/>
+      <c r="M20" s="5" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
+      <c r="A21" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C21" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D21" s="2">
+      <c r="D21" s="1">
         <v>2011</v>
       </c>
-      <c r="E21" s="8" t="s">
+      <c r="E21" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="F21" s="8"/>
-      <c r="G21" s="8"/>
-      <c r="H21" s="8"/>
-      <c r="I21" s="8"/>
-      <c r="J21" s="8"/>
-      <c r="K21" s="8"/>
-      <c r="L21" s="8"/>
-      <c r="M21" s="9" t="s">
+      <c r="F21" s="9"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="9"/>
+      <c r="J21" s="9"/>
+      <c r="K21" s="9"/>
+      <c r="L21" s="9"/>
+      <c r="M21" s="5" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
+      <c r="A22" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C22" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D22" s="2">
+      <c r="D22" s="1">
         <v>2015</v>
       </c>
-      <c r="E22" s="8" t="s">
+      <c r="E22" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="F22" s="8"/>
-      <c r="G22" s="8"/>
-      <c r="H22" s="8"/>
-      <c r="I22" s="8"/>
-      <c r="J22" s="8"/>
-      <c r="K22" s="8"/>
-      <c r="L22" s="8"/>
-      <c r="M22" s="9" t="s">
+      <c r="F22" s="9"/>
+      <c r="G22" s="9"/>
+      <c r="H22" s="9"/>
+      <c r="I22" s="9"/>
+      <c r="J22" s="9"/>
+      <c r="K22" s="9"/>
+      <c r="L22" s="9"/>
+      <c r="M22" s="5" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
+      <c r="A23" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B23" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C23" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="D23" s="2">
+      <c r="D23" s="1">
         <v>2017</v>
       </c>
-      <c r="E23" s="8" t="s">
+      <c r="E23" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="F23" s="8"/>
-      <c r="G23" s="8"/>
-      <c r="H23" s="8"/>
-      <c r="I23" s="8"/>
-      <c r="J23" s="8"/>
-      <c r="K23" s="8"/>
-      <c r="L23" s="8"/>
-      <c r="M23" s="9" t="s">
+      <c r="F23" s="9"/>
+      <c r="G23" s="9"/>
+      <c r="H23" s="9"/>
+      <c r="I23" s="9"/>
+      <c r="J23" s="9"/>
+      <c r="K23" s="9"/>
+      <c r="L23" s="9"/>
+      <c r="M23" s="5" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
+      <c r="A24" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="C24" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D24" s="2">
+      <c r="D24" s="1">
         <v>2013</v>
       </c>
-      <c r="E24" s="8" t="s">
+      <c r="E24" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="F24" s="8"/>
-      <c r="G24" s="8"/>
-      <c r="H24" s="8"/>
-      <c r="I24" s="8"/>
-      <c r="J24" s="8"/>
-      <c r="K24" s="8"/>
-      <c r="L24" s="8"/>
-      <c r="M24" s="9" t="s">
+      <c r="F24" s="9"/>
+      <c r="G24" s="9"/>
+      <c r="H24" s="9"/>
+      <c r="I24" s="9"/>
+      <c r="J24" s="9"/>
+      <c r="K24" s="9"/>
+      <c r="L24" s="9"/>
+      <c r="M24" s="5" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
+      <c r="A25" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B25" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="C25" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="D25" s="2">
+      <c r="D25" s="1">
         <v>2015</v>
       </c>
-      <c r="E25" s="8" t="s">
+      <c r="E25" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="F25" s="8"/>
-      <c r="G25" s="8"/>
-      <c r="H25" s="8"/>
-      <c r="I25" s="8"/>
-      <c r="J25" s="8"/>
-      <c r="K25" s="8"/>
-      <c r="L25" s="8"/>
-      <c r="M25" s="9" t="s">
+      <c r="F25" s="9"/>
+      <c r="G25" s="9"/>
+      <c r="H25" s="9"/>
+      <c r="I25" s="9"/>
+      <c r="J25" s="9"/>
+      <c r="K25" s="9"/>
+      <c r="L25" s="9"/>
+      <c r="M25" s="5" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
+      <c r="A26" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B26" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="C26" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D26" s="2">
+      <c r="D26" s="1">
         <v>2014</v>
       </c>
-      <c r="E26" s="8" t="s">
+      <c r="E26" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="F26" s="8"/>
-      <c r="G26" s="8"/>
-      <c r="H26" s="8"/>
-      <c r="I26" s="8"/>
-      <c r="J26" s="8"/>
-      <c r="K26" s="8"/>
-      <c r="L26" s="8"/>
-      <c r="M26" s="9" t="s">
+      <c r="F26" s="9"/>
+      <c r="G26" s="9"/>
+      <c r="H26" s="9"/>
+      <c r="I26" s="9"/>
+      <c r="J26" s="9"/>
+      <c r="K26" s="9"/>
+      <c r="L26" s="9"/>
+      <c r="M26" s="5" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
+      <c r="A27" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B27" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="C27" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D27" s="2">
+      <c r="D27" s="1">
         <v>2008</v>
       </c>
-      <c r="E27" s="8" t="s">
+      <c r="E27" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="F27" s="8"/>
-      <c r="G27" s="8"/>
-      <c r="H27" s="8"/>
-      <c r="I27" s="8"/>
-      <c r="J27" s="8"/>
-      <c r="K27" s="8"/>
-      <c r="L27" s="8"/>
-      <c r="M27" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="N27" s="2">
+      <c r="F27" s="9"/>
+      <c r="G27" s="9"/>
+      <c r="H27" s="9"/>
+      <c r="I27" s="9"/>
+      <c r="J27" s="9"/>
+      <c r="K27" s="9"/>
+      <c r="L27" s="9"/>
+      <c r="M27" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="N27" s="1">
         <v>17</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
+      <c r="A28" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B28" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="C28" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="D28" s="2">
+      <c r="D28" s="1">
         <v>2015</v>
       </c>
-      <c r="E28" s="8" t="s">
+      <c r="E28" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="F28" s="8"/>
-      <c r="G28" s="8"/>
-      <c r="H28" s="8"/>
-      <c r="I28" s="8"/>
-      <c r="J28" s="8"/>
-      <c r="K28" s="8"/>
-      <c r="L28" s="8"/>
-      <c r="M28" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="N28" s="2">
+      <c r="F28" s="9"/>
+      <c r="G28" s="9"/>
+      <c r="H28" s="9"/>
+      <c r="I28" s="9"/>
+      <c r="J28" s="9"/>
+      <c r="K28" s="9"/>
+      <c r="L28" s="9"/>
+      <c r="M28" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="N28" s="1">
         <v>15</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
+      <c r="A29" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B29" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="C29" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="D29" s="2">
+      <c r="D29" s="1">
         <v>2016</v>
       </c>
-      <c r="E29" s="8" t="s">
+      <c r="E29" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="F29" s="8"/>
-      <c r="G29" s="8"/>
-      <c r="H29" s="8"/>
-      <c r="I29" s="8"/>
-      <c r="J29" s="8"/>
-      <c r="K29" s="8"/>
-      <c r="L29" s="8"/>
-      <c r="M29" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="N29" s="2">
+      <c r="F29" s="9"/>
+      <c r="G29" s="9"/>
+      <c r="H29" s="9"/>
+      <c r="I29" s="9"/>
+      <c r="J29" s="9"/>
+      <c r="K29" s="9"/>
+      <c r="L29" s="9"/>
+      <c r="M29" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="N29" s="1">
         <v>14</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
+      <c r="A30" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B30" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="C30" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="D30" s="2">
+      <c r="D30" s="1">
         <v>1996</v>
       </c>
-      <c r="E30" s="8" t="s">
+      <c r="E30" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="F30" s="8"/>
-      <c r="G30" s="8"/>
-      <c r="H30" s="8"/>
-      <c r="I30" s="8"/>
-      <c r="J30" s="8"/>
-      <c r="K30" s="8"/>
-      <c r="L30" s="8"/>
-      <c r="M30" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="N30" s="2">
+      <c r="F30" s="9"/>
+      <c r="G30" s="9"/>
+      <c r="H30" s="9"/>
+      <c r="I30" s="9"/>
+      <c r="J30" s="9"/>
+      <c r="K30" s="9"/>
+      <c r="L30" s="9"/>
+      <c r="M30" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="N30" s="1">
         <v>16</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
+      <c r="A31" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B31" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="C31" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D31" s="2">
+      <c r="D31" s="1">
         <v>1993</v>
       </c>
-      <c r="E31" s="8" t="s">
+      <c r="E31" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="F31" s="8"/>
-      <c r="G31" s="8"/>
-      <c r="H31" s="8"/>
-      <c r="I31" s="8"/>
-      <c r="J31" s="8"/>
-      <c r="K31" s="8"/>
-      <c r="L31" s="8"/>
-      <c r="M31" s="9" t="s">
+      <c r="F31" s="9"/>
+      <c r="G31" s="9"/>
+      <c r="H31" s="9"/>
+      <c r="I31" s="9"/>
+      <c r="J31" s="9"/>
+      <c r="K31" s="9"/>
+      <c r="L31" s="9"/>
+      <c r="M31" s="5" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
+      <c r="A32" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="M32" s="5" t="s">
+      <c r="M32" s="4" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
+      <c r="A33" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="B33" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="C33" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D33" s="2">
+      <c r="D33" s="1">
         <v>2009</v>
       </c>
-      <c r="E33" s="8" t="s">
+      <c r="E33" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="F33" s="8"/>
-      <c r="G33" s="8"/>
-      <c r="H33" s="8"/>
-      <c r="I33" s="8"/>
-      <c r="J33" s="8"/>
-      <c r="K33" s="8"/>
-      <c r="L33" s="8"/>
-      <c r="M33" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="N33" s="2">
+      <c r="F33" s="9"/>
+      <c r="G33" s="9"/>
+      <c r="H33" s="9"/>
+      <c r="I33" s="9"/>
+      <c r="J33" s="9"/>
+      <c r="K33" s="9"/>
+      <c r="L33" s="9"/>
+      <c r="M33" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="N33" s="1">
         <v>13</v>
       </c>
     </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D34" s="1">
+        <v>2013</v>
+      </c>
+      <c r="E34" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="F34" s="9"/>
+      <c r="G34" s="9"/>
+      <c r="H34" s="9"/>
+      <c r="I34" s="9"/>
+      <c r="J34" s="9"/>
+      <c r="K34" s="9"/>
+      <c r="L34" s="9"/>
+      <c r="M34" s="13" t="s">
+        <v>91</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="31">
+  <mergeCells count="32">
+    <mergeCell ref="E34:L34"/>
+    <mergeCell ref="E13:L13"/>
+    <mergeCell ref="A2:M2"/>
+    <mergeCell ref="E3:L3"/>
+    <mergeCell ref="E4:L4"/>
+    <mergeCell ref="E5:L5"/>
+    <mergeCell ref="E6:L6"/>
+    <mergeCell ref="E7:L7"/>
+    <mergeCell ref="E8:L8"/>
+    <mergeCell ref="E9:L9"/>
+    <mergeCell ref="E10:L10"/>
+    <mergeCell ref="E11:L11"/>
+    <mergeCell ref="E12:L12"/>
+    <mergeCell ref="E25:L25"/>
+    <mergeCell ref="E14:L14"/>
+    <mergeCell ref="E15:L15"/>
+    <mergeCell ref="E16:L16"/>
+    <mergeCell ref="E17:L17"/>
+    <mergeCell ref="E18:L18"/>
+    <mergeCell ref="E19:L19"/>
+    <mergeCell ref="E20:L20"/>
+    <mergeCell ref="E21:L21"/>
+    <mergeCell ref="E22:L22"/>
+    <mergeCell ref="E23:L23"/>
+    <mergeCell ref="E24:L24"/>
     <mergeCell ref="E33:L33"/>
     <mergeCell ref="E26:L26"/>
     <mergeCell ref="E27:L27"/>
@@ -1619,30 +1692,6 @@
     <mergeCell ref="E30:L30"/>
     <mergeCell ref="E28:L28"/>
     <mergeCell ref="E31:L31"/>
-    <mergeCell ref="E20:L20"/>
-    <mergeCell ref="E21:L21"/>
-    <mergeCell ref="E22:L22"/>
-    <mergeCell ref="E23:L23"/>
-    <mergeCell ref="E24:L24"/>
-    <mergeCell ref="E25:L25"/>
-    <mergeCell ref="E14:L14"/>
-    <mergeCell ref="E15:L15"/>
-    <mergeCell ref="E16:L16"/>
-    <mergeCell ref="E17:L17"/>
-    <mergeCell ref="E18:L18"/>
-    <mergeCell ref="E19:L19"/>
-    <mergeCell ref="E8:L8"/>
-    <mergeCell ref="E9:L9"/>
-    <mergeCell ref="E10:L10"/>
-    <mergeCell ref="E11:L11"/>
-    <mergeCell ref="E12:L12"/>
-    <mergeCell ref="E13:L13"/>
-    <mergeCell ref="A2:M2"/>
-    <mergeCell ref="E3:L3"/>
-    <mergeCell ref="E4:L4"/>
-    <mergeCell ref="E5:L5"/>
-    <mergeCell ref="E6:L6"/>
-    <mergeCell ref="E7:L7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
8 de junho - inesc
</commit_message>
<xml_diff>
--- a/mieec-distrib-v2014/outras_cenas/referencias.xlsx
+++ b/mieec-distrib-v2014/outras_cenas/referencias.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17726"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marisa Oliveira\Documents\GitHub\Master-Thesis\mieec-distrib-v2014\outras_cenas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marisa\Master-Thesis\mieec-distrib-v2014\outras_cenas\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="95">
   <si>
     <t>REF</t>
   </si>
@@ -303,6 +303,12 @@
   </si>
   <si>
     <t>Implementing SMPTE SDI Interfaces with 7 Series Transceivers</t>
+  </si>
+  <si>
+    <t>R032</t>
+  </si>
+  <si>
+    <t>High-Speed Serial I/0 Made Simple</t>
   </si>
 </sst>
 </file>
@@ -442,6 +448,9 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -452,9 +461,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -738,10 +744,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N34"/>
+  <dimension ref="A1:N35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34:L34"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -761,21 +767,21 @@
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
-      <c r="K2" s="10"/>
-      <c r="L2" s="10"/>
-      <c r="M2" s="10"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="11"/>
+      <c r="M2" s="11"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
@@ -790,16 +796,16 @@
       <c r="D3" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E3" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="11"/>
-      <c r="J3" s="11"/>
-      <c r="K3" s="11"/>
-      <c r="L3" s="11"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="12"/>
+      <c r="K3" s="12"/>
+      <c r="L3" s="12"/>
       <c r="M3" s="3" t="s">
         <v>4</v>
       </c>
@@ -817,16 +823,16 @@
       <c r="C4" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E4" s="12" t="s">
+      <c r="E4" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
-      <c r="J4" s="12"/>
-      <c r="K4" s="12"/>
-      <c r="L4" s="12"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13"/>
+      <c r="J4" s="13"/>
+      <c r="K4" s="13"/>
+      <c r="L4" s="13"/>
       <c r="M4" s="8" t="s">
         <v>37</v>
       </c>
@@ -841,16 +847,16 @@
       <c r="C5" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="E5" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
-      <c r="J5" s="9"/>
-      <c r="K5" s="9"/>
-      <c r="L5" s="9"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="10"/>
+      <c r="L5" s="10"/>
       <c r="M5" s="6" t="s">
         <v>37</v>
       </c>
@@ -868,16 +874,16 @@
       <c r="C6" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="E6" s="9" t="s">
+      <c r="E6" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="9"/>
-      <c r="J6" s="9"/>
-      <c r="K6" s="9"/>
-      <c r="L6" s="9"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="10"/>
+      <c r="K6" s="10"/>
+      <c r="L6" s="10"/>
       <c r="M6" s="5" t="s">
         <v>44</v>
       </c>
@@ -892,16 +898,16 @@
       <c r="C7" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="E7" s="9" t="s">
+      <c r="E7" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="9"/>
-      <c r="J7" s="9"/>
-      <c r="K7" s="9"/>
-      <c r="L7" s="9"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="10"/>
+      <c r="K7" s="10"/>
+      <c r="L7" s="10"/>
       <c r="M7" s="5" t="s">
         <v>37</v>
       </c>
@@ -919,16 +925,16 @@
       <c r="C8" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="E8" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9"/>
-      <c r="J8" s="9"/>
-      <c r="K8" s="9"/>
-      <c r="L8" s="9"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10"/>
+      <c r="K8" s="10"/>
+      <c r="L8" s="10"/>
       <c r="M8" s="6" t="s">
         <v>37</v>
       </c>
@@ -946,16 +952,16 @@
       <c r="C9" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E9" s="9" t="s">
+      <c r="E9" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="9"/>
-      <c r="J9" s="9"/>
-      <c r="K9" s="9"/>
-      <c r="L9" s="9"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="10"/>
       <c r="M9" s="5" t="s">
         <v>37</v>
       </c>
@@ -973,16 +979,16 @@
       <c r="D10" s="1">
         <v>2014</v>
       </c>
-      <c r="E10" s="9" t="s">
+      <c r="E10" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="9"/>
-      <c r="K10" s="9"/>
-      <c r="L10" s="9"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="10"/>
+      <c r="L10" s="10"/>
       <c r="M10" s="6" t="s">
         <v>37</v>
       </c>
@@ -1003,16 +1009,16 @@
       <c r="D11" s="1">
         <v>2014</v>
       </c>
-      <c r="E11" s="9" t="s">
+      <c r="E11" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="9"/>
-      <c r="I11" s="9"/>
-      <c r="J11" s="9"/>
-      <c r="K11" s="9"/>
-      <c r="L11" s="9"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="10"/>
+      <c r="L11" s="10"/>
       <c r="M11" s="6" t="s">
         <v>37</v>
       </c>
@@ -1033,16 +1039,16 @@
       <c r="D12" s="1">
         <v>2014</v>
       </c>
-      <c r="E12" s="9" t="s">
+      <c r="E12" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="9"/>
-      <c r="I12" s="9"/>
-      <c r="J12" s="9"/>
-      <c r="K12" s="9"/>
-      <c r="L12" s="9"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="10"/>
+      <c r="J12" s="10"/>
+      <c r="K12" s="10"/>
+      <c r="L12" s="10"/>
       <c r="M12" s="6" t="s">
         <v>37</v>
       </c>
@@ -1063,16 +1069,16 @@
       <c r="D13" s="1">
         <v>2013</v>
       </c>
-      <c r="E13" s="9" t="s">
+      <c r="E13" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
-      <c r="H13" s="9"/>
-      <c r="I13" s="9"/>
-      <c r="J13" s="9"/>
-      <c r="K13" s="9"/>
-      <c r="L13" s="9"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="10"/>
+      <c r="K13" s="10"/>
+      <c r="L13" s="10"/>
       <c r="M13" s="6" t="s">
         <v>37</v>
       </c>
@@ -1093,16 +1099,16 @@
       <c r="D14" s="1">
         <v>2016</v>
       </c>
-      <c r="E14" s="9" t="s">
+      <c r="E14" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9"/>
-      <c r="H14" s="9"/>
-      <c r="I14" s="9"/>
-      <c r="J14" s="9"/>
-      <c r="K14" s="9"/>
-      <c r="L14" s="9"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="10"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="10"/>
+      <c r="K14" s="10"/>
+      <c r="L14" s="10"/>
       <c r="M14" s="6" t="s">
         <v>37</v>
       </c>
@@ -1123,16 +1129,16 @@
       <c r="D15" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="E15" s="9" t="s">
+      <c r="E15" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="F15" s="9"/>
-      <c r="G15" s="9"/>
-      <c r="H15" s="9"/>
-      <c r="I15" s="9"/>
-      <c r="J15" s="9"/>
-      <c r="K15" s="9"/>
-      <c r="L15" s="9"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="10"/>
+      <c r="K15" s="10"/>
+      <c r="L15" s="10"/>
       <c r="M15" s="6" t="s">
         <v>37</v>
       </c>
@@ -1153,16 +1159,16 @@
       <c r="D16" s="1">
         <v>2015</v>
       </c>
-      <c r="E16" s="9" t="s">
+      <c r="E16" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="F16" s="9"/>
-      <c r="G16" s="9"/>
-      <c r="H16" s="9"/>
-      <c r="I16" s="9"/>
-      <c r="J16" s="9"/>
-      <c r="K16" s="9"/>
-      <c r="L16" s="9"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="10"/>
+      <c r="J16" s="10"/>
+      <c r="K16" s="10"/>
+      <c r="L16" s="10"/>
       <c r="M16" s="6" t="s">
         <v>37</v>
       </c>
@@ -1183,16 +1189,16 @@
       <c r="D17" s="1">
         <v>2014</v>
       </c>
-      <c r="E17" s="9" t="s">
+      <c r="E17" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="F17" s="9"/>
-      <c r="G17" s="9"/>
-      <c r="H17" s="9"/>
-      <c r="I17" s="9"/>
-      <c r="J17" s="9"/>
-      <c r="K17" s="9"/>
-      <c r="L17" s="9"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="10"/>
+      <c r="I17" s="10"/>
+      <c r="J17" s="10"/>
+      <c r="K17" s="10"/>
+      <c r="L17" s="10"/>
       <c r="M17" s="6" t="s">
         <v>37</v>
       </c>
@@ -1213,16 +1219,16 @@
       <c r="D18" s="1">
         <v>2016</v>
       </c>
-      <c r="E18" s="9" t="s">
+      <c r="E18" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="F18" s="9"/>
-      <c r="G18" s="9"/>
-      <c r="H18" s="9"/>
-      <c r="I18" s="9"/>
-      <c r="J18" s="9"/>
-      <c r="K18" s="9"/>
-      <c r="L18" s="9"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="10"/>
+      <c r="I18" s="10"/>
+      <c r="J18" s="10"/>
+      <c r="K18" s="10"/>
+      <c r="L18" s="10"/>
       <c r="M18" s="5" t="s">
         <v>37</v>
       </c>
@@ -1240,16 +1246,16 @@
       <c r="D19" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="E19" s="9" t="s">
+      <c r="E19" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="F19" s="9"/>
-      <c r="G19" s="9"/>
-      <c r="H19" s="9"/>
-      <c r="I19" s="9"/>
-      <c r="J19" s="9"/>
-      <c r="K19" s="9"/>
-      <c r="L19" s="9"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="10"/>
+      <c r="H19" s="10"/>
+      <c r="I19" s="10"/>
+      <c r="J19" s="10"/>
+      <c r="K19" s="10"/>
+      <c r="L19" s="10"/>
       <c r="M19" s="6" t="s">
         <v>37</v>
       </c>
@@ -1270,16 +1276,16 @@
       <c r="D20" s="1">
         <v>2012</v>
       </c>
-      <c r="E20" s="9" t="s">
+      <c r="E20" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="F20" s="9"/>
-      <c r="G20" s="9"/>
-      <c r="H20" s="9"/>
-      <c r="I20" s="9"/>
-      <c r="J20" s="9"/>
-      <c r="K20" s="9"/>
-      <c r="L20" s="9"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="10"/>
+      <c r="H20" s="10"/>
+      <c r="I20" s="10"/>
+      <c r="J20" s="10"/>
+      <c r="K20" s="10"/>
+      <c r="L20" s="10"/>
       <c r="M20" s="5" t="s">
         <v>37</v>
       </c>
@@ -1297,16 +1303,16 @@
       <c r="D21" s="1">
         <v>2011</v>
       </c>
-      <c r="E21" s="9" t="s">
+      <c r="E21" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="F21" s="9"/>
-      <c r="G21" s="9"/>
-      <c r="H21" s="9"/>
-      <c r="I21" s="9"/>
-      <c r="J21" s="9"/>
-      <c r="K21" s="9"/>
-      <c r="L21" s="9"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="10"/>
+      <c r="H21" s="10"/>
+      <c r="I21" s="10"/>
+      <c r="J21" s="10"/>
+      <c r="K21" s="10"/>
+      <c r="L21" s="10"/>
       <c r="M21" s="5" t="s">
         <v>37</v>
       </c>
@@ -1324,16 +1330,16 @@
       <c r="D22" s="1">
         <v>2015</v>
       </c>
-      <c r="E22" s="9" t="s">
+      <c r="E22" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="F22" s="9"/>
-      <c r="G22" s="9"/>
-      <c r="H22" s="9"/>
-      <c r="I22" s="9"/>
-      <c r="J22" s="9"/>
-      <c r="K22" s="9"/>
-      <c r="L22" s="9"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="10"/>
+      <c r="H22" s="10"/>
+      <c r="I22" s="10"/>
+      <c r="J22" s="10"/>
+      <c r="K22" s="10"/>
+      <c r="L22" s="10"/>
       <c r="M22" s="5" t="s">
         <v>37</v>
       </c>
@@ -1351,16 +1357,16 @@
       <c r="D23" s="1">
         <v>2017</v>
       </c>
-      <c r="E23" s="9" t="s">
+      <c r="E23" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="F23" s="9"/>
-      <c r="G23" s="9"/>
-      <c r="H23" s="9"/>
-      <c r="I23" s="9"/>
-      <c r="J23" s="9"/>
-      <c r="K23" s="9"/>
-      <c r="L23" s="9"/>
+      <c r="F23" s="10"/>
+      <c r="G23" s="10"/>
+      <c r="H23" s="10"/>
+      <c r="I23" s="10"/>
+      <c r="J23" s="10"/>
+      <c r="K23" s="10"/>
+      <c r="L23" s="10"/>
       <c r="M23" s="5" t="s">
         <v>37</v>
       </c>
@@ -1378,16 +1384,16 @@
       <c r="D24" s="1">
         <v>2013</v>
       </c>
-      <c r="E24" s="9" t="s">
+      <c r="E24" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="F24" s="9"/>
-      <c r="G24" s="9"/>
-      <c r="H24" s="9"/>
-      <c r="I24" s="9"/>
-      <c r="J24" s="9"/>
-      <c r="K24" s="9"/>
-      <c r="L24" s="9"/>
+      <c r="F24" s="10"/>
+      <c r="G24" s="10"/>
+      <c r="H24" s="10"/>
+      <c r="I24" s="10"/>
+      <c r="J24" s="10"/>
+      <c r="K24" s="10"/>
+      <c r="L24" s="10"/>
       <c r="M24" s="5" t="s">
         <v>37</v>
       </c>
@@ -1405,16 +1411,16 @@
       <c r="D25" s="1">
         <v>2015</v>
       </c>
-      <c r="E25" s="9" t="s">
+      <c r="E25" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="F25" s="9"/>
-      <c r="G25" s="9"/>
-      <c r="H25" s="9"/>
-      <c r="I25" s="9"/>
-      <c r="J25" s="9"/>
-      <c r="K25" s="9"/>
-      <c r="L25" s="9"/>
+      <c r="F25" s="10"/>
+      <c r="G25" s="10"/>
+      <c r="H25" s="10"/>
+      <c r="I25" s="10"/>
+      <c r="J25" s="10"/>
+      <c r="K25" s="10"/>
+      <c r="L25" s="10"/>
       <c r="M25" s="5" t="s">
         <v>37</v>
       </c>
@@ -1432,16 +1438,16 @@
       <c r="D26" s="1">
         <v>2014</v>
       </c>
-      <c r="E26" s="9" t="s">
+      <c r="E26" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="F26" s="9"/>
-      <c r="G26" s="9"/>
-      <c r="H26" s="9"/>
-      <c r="I26" s="9"/>
-      <c r="J26" s="9"/>
-      <c r="K26" s="9"/>
-      <c r="L26" s="9"/>
+      <c r="F26" s="10"/>
+      <c r="G26" s="10"/>
+      <c r="H26" s="10"/>
+      <c r="I26" s="10"/>
+      <c r="J26" s="10"/>
+      <c r="K26" s="10"/>
+      <c r="L26" s="10"/>
       <c r="M26" s="5" t="s">
         <v>37</v>
       </c>
@@ -1459,16 +1465,16 @@
       <c r="D27" s="1">
         <v>2008</v>
       </c>
-      <c r="E27" s="9" t="s">
+      <c r="E27" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="F27" s="9"/>
-      <c r="G27" s="9"/>
-      <c r="H27" s="9"/>
-      <c r="I27" s="9"/>
-      <c r="J27" s="9"/>
-      <c r="K27" s="9"/>
-      <c r="L27" s="9"/>
+      <c r="F27" s="10"/>
+      <c r="G27" s="10"/>
+      <c r="H27" s="10"/>
+      <c r="I27" s="10"/>
+      <c r="J27" s="10"/>
+      <c r="K27" s="10"/>
+      <c r="L27" s="10"/>
       <c r="M27" s="6" t="s">
         <v>37</v>
       </c>
@@ -1489,16 +1495,16 @@
       <c r="D28" s="1">
         <v>2015</v>
       </c>
-      <c r="E28" s="9" t="s">
+      <c r="E28" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="F28" s="9"/>
-      <c r="G28" s="9"/>
-      <c r="H28" s="9"/>
-      <c r="I28" s="9"/>
-      <c r="J28" s="9"/>
-      <c r="K28" s="9"/>
-      <c r="L28" s="9"/>
+      <c r="F28" s="10"/>
+      <c r="G28" s="10"/>
+      <c r="H28" s="10"/>
+      <c r="I28" s="10"/>
+      <c r="J28" s="10"/>
+      <c r="K28" s="10"/>
+      <c r="L28" s="10"/>
       <c r="M28" s="6" t="s">
         <v>37</v>
       </c>
@@ -1519,16 +1525,16 @@
       <c r="D29" s="1">
         <v>2016</v>
       </c>
-      <c r="E29" s="9" t="s">
+      <c r="E29" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="F29" s="9"/>
-      <c r="G29" s="9"/>
-      <c r="H29" s="9"/>
-      <c r="I29" s="9"/>
-      <c r="J29" s="9"/>
-      <c r="K29" s="9"/>
-      <c r="L29" s="9"/>
+      <c r="F29" s="10"/>
+      <c r="G29" s="10"/>
+      <c r="H29" s="10"/>
+      <c r="I29" s="10"/>
+      <c r="J29" s="10"/>
+      <c r="K29" s="10"/>
+      <c r="L29" s="10"/>
       <c r="M29" s="6" t="s">
         <v>37</v>
       </c>
@@ -1549,16 +1555,16 @@
       <c r="D30" s="1">
         <v>1996</v>
       </c>
-      <c r="E30" s="9" t="s">
+      <c r="E30" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="F30" s="9"/>
-      <c r="G30" s="9"/>
-      <c r="H30" s="9"/>
-      <c r="I30" s="9"/>
-      <c r="J30" s="9"/>
-      <c r="K30" s="9"/>
-      <c r="L30" s="9"/>
+      <c r="F30" s="10"/>
+      <c r="G30" s="10"/>
+      <c r="H30" s="10"/>
+      <c r="I30" s="10"/>
+      <c r="J30" s="10"/>
+      <c r="K30" s="10"/>
+      <c r="L30" s="10"/>
       <c r="M30" s="6" t="s">
         <v>37</v>
       </c>
@@ -1579,16 +1585,16 @@
       <c r="D31" s="1">
         <v>1993</v>
       </c>
-      <c r="E31" s="9" t="s">
+      <c r="E31" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="F31" s="9"/>
-      <c r="G31" s="9"/>
-      <c r="H31" s="9"/>
-      <c r="I31" s="9"/>
-      <c r="J31" s="9"/>
-      <c r="K31" s="9"/>
-      <c r="L31" s="9"/>
+      <c r="F31" s="10"/>
+      <c r="G31" s="10"/>
+      <c r="H31" s="10"/>
+      <c r="I31" s="10"/>
+      <c r="J31" s="10"/>
+      <c r="K31" s="10"/>
+      <c r="L31" s="10"/>
       <c r="M31" s="5" t="s">
         <v>37</v>
       </c>
@@ -1614,16 +1620,16 @@
       <c r="D33" s="1">
         <v>2009</v>
       </c>
-      <c r="E33" s="9" t="s">
+      <c r="E33" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="F33" s="9"/>
-      <c r="G33" s="9"/>
-      <c r="H33" s="9"/>
-      <c r="I33" s="9"/>
-      <c r="J33" s="9"/>
-      <c r="K33" s="9"/>
-      <c r="L33" s="9"/>
+      <c r="F33" s="10"/>
+      <c r="G33" s="10"/>
+      <c r="H33" s="10"/>
+      <c r="I33" s="10"/>
+      <c r="J33" s="10"/>
+      <c r="K33" s="10"/>
+      <c r="L33" s="10"/>
       <c r="M33" s="6" t="s">
         <v>37</v>
       </c>
@@ -1644,22 +1650,66 @@
       <c r="D34" s="1">
         <v>2013</v>
       </c>
-      <c r="E34" s="9" t="s">
+      <c r="E34" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="F34" s="9"/>
-      <c r="G34" s="9"/>
-      <c r="H34" s="9"/>
-      <c r="I34" s="9"/>
-      <c r="J34" s="9"/>
-      <c r="K34" s="9"/>
-      <c r="L34" s="9"/>
-      <c r="M34" s="13" t="s">
+      <c r="F34" s="10"/>
+      <c r="G34" s="10"/>
+      <c r="H34" s="10"/>
+      <c r="I34" s="10"/>
+      <c r="J34" s="10"/>
+      <c r="K34" s="10"/>
+      <c r="L34" s="10"/>
+      <c r="M34" s="9" t="s">
         <v>91</v>
       </c>
     </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D35" s="1">
+        <v>2005</v>
+      </c>
+      <c r="E35" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="F35" s="10"/>
+      <c r="G35" s="10"/>
+      <c r="H35" s="10"/>
+      <c r="I35" s="10"/>
+      <c r="J35" s="10"/>
+      <c r="K35" s="10"/>
+      <c r="L35" s="10"/>
+      <c r="M35" s="9" t="s">
+        <v>37</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="32">
+  <mergeCells count="33">
+    <mergeCell ref="E35:L35"/>
+    <mergeCell ref="E21:L21"/>
+    <mergeCell ref="E22:L22"/>
+    <mergeCell ref="E23:L23"/>
+    <mergeCell ref="E24:L24"/>
+    <mergeCell ref="E33:L33"/>
+    <mergeCell ref="E26:L26"/>
+    <mergeCell ref="E27:L27"/>
+    <mergeCell ref="E29:L29"/>
+    <mergeCell ref="E30:L30"/>
+    <mergeCell ref="E28:L28"/>
+    <mergeCell ref="E31:L31"/>
+    <mergeCell ref="E16:L16"/>
+    <mergeCell ref="E17:L17"/>
+    <mergeCell ref="E18:L18"/>
+    <mergeCell ref="E19:L19"/>
+    <mergeCell ref="E20:L20"/>
     <mergeCell ref="E34:L34"/>
     <mergeCell ref="E13:L13"/>
     <mergeCell ref="A2:M2"/>
@@ -1676,22 +1726,6 @@
     <mergeCell ref="E25:L25"/>
     <mergeCell ref="E14:L14"/>
     <mergeCell ref="E15:L15"/>
-    <mergeCell ref="E16:L16"/>
-    <mergeCell ref="E17:L17"/>
-    <mergeCell ref="E18:L18"/>
-    <mergeCell ref="E19:L19"/>
-    <mergeCell ref="E20:L20"/>
-    <mergeCell ref="E21:L21"/>
-    <mergeCell ref="E22:L22"/>
-    <mergeCell ref="E23:L23"/>
-    <mergeCell ref="E24:L24"/>
-    <mergeCell ref="E33:L33"/>
-    <mergeCell ref="E26:L26"/>
-    <mergeCell ref="E27:L27"/>
-    <mergeCell ref="E29:L29"/>
-    <mergeCell ref="E30:L30"/>
-    <mergeCell ref="E28:L28"/>
-    <mergeCell ref="E31:L31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
Algumas correcções do capitulo 3
</commit_message>
<xml_diff>
--- a/mieec-distrib-v2014/outras_cenas/referencias.xlsx
+++ b/mieec-distrib-v2014/outras_cenas/referencias.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17726"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marisa\Master-Thesis\mieec-distrib-v2014\outras_cenas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marisa Oliveira\Documents\GitHub\Master-Thesis\mieec-distrib-v2014\outras_cenas\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="109">
   <si>
     <t>REF</t>
   </si>
@@ -309,6 +309,48 @@
   </si>
   <si>
     <t>High-Speed Serial I/0 Made Simple</t>
+  </si>
+  <si>
+    <t>R033</t>
+  </si>
+  <si>
+    <t>R034</t>
+  </si>
+  <si>
+    <t>R035</t>
+  </si>
+  <si>
+    <t>R036</t>
+  </si>
+  <si>
+    <t>R037</t>
+  </si>
+  <si>
+    <t>R038</t>
+  </si>
+  <si>
+    <t>R039</t>
+  </si>
+  <si>
+    <t>Data Sheet de ADV7511</t>
+  </si>
+  <si>
+    <t>Data Sheet de ADV612</t>
+  </si>
+  <si>
+    <t>Understanding Metastability in FPGAs</t>
+  </si>
+  <si>
+    <t>LVDS Owner's Manual</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Single-Ended vs Differential Inputs - </t>
+  </si>
+  <si>
+    <t>The Shift Register</t>
+  </si>
+  <si>
+    <t>A 1 . 25Gbit / s Serializer for LHC Data and Trigger Optical Links</t>
   </si>
 </sst>
 </file>
@@ -422,7 +464,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -455,12 +497,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -744,10 +792,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N35"/>
+  <dimension ref="A1:N42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -767,21 +815,21 @@
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
-      <c r="K2" s="11"/>
-      <c r="L2" s="11"/>
-      <c r="M2" s="11"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
+      <c r="K2" s="12"/>
+      <c r="L2" s="12"/>
+      <c r="M2" s="12"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
@@ -796,16 +844,16 @@
       <c r="D3" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="E3" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="12"/>
-      <c r="J3" s="12"/>
-      <c r="K3" s="12"/>
-      <c r="L3" s="12"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="13"/>
+      <c r="J3" s="13"/>
+      <c r="K3" s="13"/>
+      <c r="L3" s="13"/>
       <c r="M3" s="3" t="s">
         <v>4</v>
       </c>
@@ -823,16 +871,16 @@
       <c r="C4" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E4" s="13" t="s">
+      <c r="E4" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13"/>
-      <c r="J4" s="13"/>
-      <c r="K4" s="13"/>
-      <c r="L4" s="13"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="14"/>
+      <c r="L4" s="14"/>
       <c r="M4" s="8" t="s">
         <v>37</v>
       </c>
@@ -847,16 +895,16 @@
       <c r="C5" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="E5" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
-      <c r="J5" s="10"/>
-      <c r="K5" s="10"/>
-      <c r="L5" s="10"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="11"/>
+      <c r="K5" s="11"/>
+      <c r="L5" s="11"/>
       <c r="M5" s="6" t="s">
         <v>37</v>
       </c>
@@ -874,16 +922,16 @@
       <c r="C6" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="E6" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10"/>
-      <c r="K6" s="10"/>
-      <c r="L6" s="10"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="11"/>
+      <c r="K6" s="11"/>
+      <c r="L6" s="11"/>
       <c r="M6" s="5" t="s">
         <v>44</v>
       </c>
@@ -898,16 +946,16 @@
       <c r="C7" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="E7" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10"/>
-      <c r="J7" s="10"/>
-      <c r="K7" s="10"/>
-      <c r="L7" s="10"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="11"/>
+      <c r="K7" s="11"/>
+      <c r="L7" s="11"/>
       <c r="M7" s="5" t="s">
         <v>37</v>
       </c>
@@ -925,16 +973,16 @@
       <c r="C8" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E8" s="10" t="s">
+      <c r="E8" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="10"/>
-      <c r="K8" s="10"/>
-      <c r="L8" s="10"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="11"/>
+      <c r="K8" s="11"/>
+      <c r="L8" s="11"/>
       <c r="M8" s="6" t="s">
         <v>37</v>
       </c>
@@ -952,16 +1000,16 @@
       <c r="C9" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E9" s="10" t="s">
+      <c r="E9" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="10"/>
-      <c r="J9" s="10"/>
-      <c r="K9" s="10"/>
-      <c r="L9" s="10"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="11"/>
+      <c r="J9" s="11"/>
+      <c r="K9" s="11"/>
+      <c r="L9" s="11"/>
       <c r="M9" s="5" t="s">
         <v>37</v>
       </c>
@@ -979,16 +1027,16 @@
       <c r="D10" s="1">
         <v>2014</v>
       </c>
-      <c r="E10" s="10" t="s">
+      <c r="E10" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="10"/>
-      <c r="I10" s="10"/>
-      <c r="J10" s="10"/>
-      <c r="K10" s="10"/>
-      <c r="L10" s="10"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="11"/>
+      <c r="J10" s="11"/>
+      <c r="K10" s="11"/>
+      <c r="L10" s="11"/>
       <c r="M10" s="6" t="s">
         <v>37</v>
       </c>
@@ -1009,16 +1057,16 @@
       <c r="D11" s="1">
         <v>2014</v>
       </c>
-      <c r="E11" s="10" t="s">
+      <c r="E11" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="10"/>
-      <c r="I11" s="10"/>
-      <c r="J11" s="10"/>
-      <c r="K11" s="10"/>
-      <c r="L11" s="10"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="11"/>
+      <c r="K11" s="11"/>
+      <c r="L11" s="11"/>
       <c r="M11" s="6" t="s">
         <v>37</v>
       </c>
@@ -1039,16 +1087,16 @@
       <c r="D12" s="1">
         <v>2014</v>
       </c>
-      <c r="E12" s="10" t="s">
+      <c r="E12" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="10"/>
-      <c r="I12" s="10"/>
-      <c r="J12" s="10"/>
-      <c r="K12" s="10"/>
-      <c r="L12" s="10"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="11"/>
+      <c r="J12" s="11"/>
+      <c r="K12" s="11"/>
+      <c r="L12" s="11"/>
       <c r="M12" s="6" t="s">
         <v>37</v>
       </c>
@@ -1069,16 +1117,16 @@
       <c r="D13" s="1">
         <v>2013</v>
       </c>
-      <c r="E13" s="10" t="s">
+      <c r="E13" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="10"/>
-      <c r="I13" s="10"/>
-      <c r="J13" s="10"/>
-      <c r="K13" s="10"/>
-      <c r="L13" s="10"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="11"/>
+      <c r="J13" s="11"/>
+      <c r="K13" s="11"/>
+      <c r="L13" s="11"/>
       <c r="M13" s="6" t="s">
         <v>37</v>
       </c>
@@ -1099,16 +1147,16 @@
       <c r="D14" s="1">
         <v>2016</v>
       </c>
-      <c r="E14" s="10" t="s">
+      <c r="E14" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="10"/>
-      <c r="I14" s="10"/>
-      <c r="J14" s="10"/>
-      <c r="K14" s="10"/>
-      <c r="L14" s="10"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="11"/>
+      <c r="J14" s="11"/>
+      <c r="K14" s="11"/>
+      <c r="L14" s="11"/>
       <c r="M14" s="6" t="s">
         <v>37</v>
       </c>
@@ -1129,16 +1177,16 @@
       <c r="D15" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="E15" s="10" t="s">
+      <c r="E15" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10"/>
-      <c r="H15" s="10"/>
-      <c r="I15" s="10"/>
-      <c r="J15" s="10"/>
-      <c r="K15" s="10"/>
-      <c r="L15" s="10"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11"/>
+      <c r="H15" s="11"/>
+      <c r="I15" s="11"/>
+      <c r="J15" s="11"/>
+      <c r="K15" s="11"/>
+      <c r="L15" s="11"/>
       <c r="M15" s="6" t="s">
         <v>37</v>
       </c>
@@ -1159,16 +1207,16 @@
       <c r="D16" s="1">
         <v>2015</v>
       </c>
-      <c r="E16" s="10" t="s">
+      <c r="E16" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="F16" s="10"/>
-      <c r="G16" s="10"/>
-      <c r="H16" s="10"/>
-      <c r="I16" s="10"/>
-      <c r="J16" s="10"/>
-      <c r="K16" s="10"/>
-      <c r="L16" s="10"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="11"/>
+      <c r="J16" s="11"/>
+      <c r="K16" s="11"/>
+      <c r="L16" s="11"/>
       <c r="M16" s="6" t="s">
         <v>37</v>
       </c>
@@ -1189,16 +1237,16 @@
       <c r="D17" s="1">
         <v>2014</v>
       </c>
-      <c r="E17" s="10" t="s">
+      <c r="E17" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="F17" s="10"/>
-      <c r="G17" s="10"/>
-      <c r="H17" s="10"/>
-      <c r="I17" s="10"/>
-      <c r="J17" s="10"/>
-      <c r="K17" s="10"/>
-      <c r="L17" s="10"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="11"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="11"/>
+      <c r="J17" s="11"/>
+      <c r="K17" s="11"/>
+      <c r="L17" s="11"/>
       <c r="M17" s="6" t="s">
         <v>37</v>
       </c>
@@ -1219,16 +1267,16 @@
       <c r="D18" s="1">
         <v>2016</v>
       </c>
-      <c r="E18" s="10" t="s">
+      <c r="E18" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="F18" s="10"/>
-      <c r="G18" s="10"/>
-      <c r="H18" s="10"/>
-      <c r="I18" s="10"/>
-      <c r="J18" s="10"/>
-      <c r="K18" s="10"/>
-      <c r="L18" s="10"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="11"/>
+      <c r="J18" s="11"/>
+      <c r="K18" s="11"/>
+      <c r="L18" s="11"/>
       <c r="M18" s="5" t="s">
         <v>37</v>
       </c>
@@ -1246,16 +1294,16 @@
       <c r="D19" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="E19" s="10" t="s">
+      <c r="E19" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="F19" s="10"/>
-      <c r="G19" s="10"/>
-      <c r="H19" s="10"/>
-      <c r="I19" s="10"/>
-      <c r="J19" s="10"/>
-      <c r="K19" s="10"/>
-      <c r="L19" s="10"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="11"/>
+      <c r="J19" s="11"/>
+      <c r="K19" s="11"/>
+      <c r="L19" s="11"/>
       <c r="M19" s="6" t="s">
         <v>37</v>
       </c>
@@ -1276,16 +1324,16 @@
       <c r="D20" s="1">
         <v>2012</v>
       </c>
-      <c r="E20" s="10" t="s">
+      <c r="E20" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="F20" s="10"/>
-      <c r="G20" s="10"/>
-      <c r="H20" s="10"/>
-      <c r="I20" s="10"/>
-      <c r="J20" s="10"/>
-      <c r="K20" s="10"/>
-      <c r="L20" s="10"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="11"/>
+      <c r="H20" s="11"/>
+      <c r="I20" s="11"/>
+      <c r="J20" s="11"/>
+      <c r="K20" s="11"/>
+      <c r="L20" s="11"/>
       <c r="M20" s="5" t="s">
         <v>37</v>
       </c>
@@ -1303,16 +1351,16 @@
       <c r="D21" s="1">
         <v>2011</v>
       </c>
-      <c r="E21" s="10" t="s">
+      <c r="E21" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="F21" s="10"/>
-      <c r="G21" s="10"/>
-      <c r="H21" s="10"/>
-      <c r="I21" s="10"/>
-      <c r="J21" s="10"/>
-      <c r="K21" s="10"/>
-      <c r="L21" s="10"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="11"/>
+      <c r="H21" s="11"/>
+      <c r="I21" s="11"/>
+      <c r="J21" s="11"/>
+      <c r="K21" s="11"/>
+      <c r="L21" s="11"/>
       <c r="M21" s="5" t="s">
         <v>37</v>
       </c>
@@ -1330,16 +1378,16 @@
       <c r="D22" s="1">
         <v>2015</v>
       </c>
-      <c r="E22" s="10" t="s">
+      <c r="E22" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="F22" s="10"/>
-      <c r="G22" s="10"/>
-      <c r="H22" s="10"/>
-      <c r="I22" s="10"/>
-      <c r="J22" s="10"/>
-      <c r="K22" s="10"/>
-      <c r="L22" s="10"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="11"/>
+      <c r="H22" s="11"/>
+      <c r="I22" s="11"/>
+      <c r="J22" s="11"/>
+      <c r="K22" s="11"/>
+      <c r="L22" s="11"/>
       <c r="M22" s="5" t="s">
         <v>37</v>
       </c>
@@ -1357,16 +1405,16 @@
       <c r="D23" s="1">
         <v>2017</v>
       </c>
-      <c r="E23" s="10" t="s">
+      <c r="E23" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="F23" s="10"/>
-      <c r="G23" s="10"/>
-      <c r="H23" s="10"/>
-      <c r="I23" s="10"/>
-      <c r="J23" s="10"/>
-      <c r="K23" s="10"/>
-      <c r="L23" s="10"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="11"/>
+      <c r="H23" s="11"/>
+      <c r="I23" s="11"/>
+      <c r="J23" s="11"/>
+      <c r="K23" s="11"/>
+      <c r="L23" s="11"/>
       <c r="M23" s="5" t="s">
         <v>37</v>
       </c>
@@ -1384,16 +1432,16 @@
       <c r="D24" s="1">
         <v>2013</v>
       </c>
-      <c r="E24" s="10" t="s">
+      <c r="E24" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="F24" s="10"/>
-      <c r="G24" s="10"/>
-      <c r="H24" s="10"/>
-      <c r="I24" s="10"/>
-      <c r="J24" s="10"/>
-      <c r="K24" s="10"/>
-      <c r="L24" s="10"/>
+      <c r="F24" s="11"/>
+      <c r="G24" s="11"/>
+      <c r="H24" s="11"/>
+      <c r="I24" s="11"/>
+      <c r="J24" s="11"/>
+      <c r="K24" s="11"/>
+      <c r="L24" s="11"/>
       <c r="M24" s="5" t="s">
         <v>37</v>
       </c>
@@ -1411,16 +1459,16 @@
       <c r="D25" s="1">
         <v>2015</v>
       </c>
-      <c r="E25" s="10" t="s">
+      <c r="E25" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="F25" s="10"/>
-      <c r="G25" s="10"/>
-      <c r="H25" s="10"/>
-      <c r="I25" s="10"/>
-      <c r="J25" s="10"/>
-      <c r="K25" s="10"/>
-      <c r="L25" s="10"/>
+      <c r="F25" s="11"/>
+      <c r="G25" s="11"/>
+      <c r="H25" s="11"/>
+      <c r="I25" s="11"/>
+      <c r="J25" s="11"/>
+      <c r="K25" s="11"/>
+      <c r="L25" s="11"/>
       <c r="M25" s="5" t="s">
         <v>37</v>
       </c>
@@ -1438,16 +1486,16 @@
       <c r="D26" s="1">
         <v>2014</v>
       </c>
-      <c r="E26" s="10" t="s">
+      <c r="E26" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="F26" s="10"/>
-      <c r="G26" s="10"/>
-      <c r="H26" s="10"/>
-      <c r="I26" s="10"/>
-      <c r="J26" s="10"/>
-      <c r="K26" s="10"/>
-      <c r="L26" s="10"/>
+      <c r="F26" s="11"/>
+      <c r="G26" s="11"/>
+      <c r="H26" s="11"/>
+      <c r="I26" s="11"/>
+      <c r="J26" s="11"/>
+      <c r="K26" s="11"/>
+      <c r="L26" s="11"/>
       <c r="M26" s="5" t="s">
         <v>37</v>
       </c>
@@ -1465,16 +1513,16 @@
       <c r="D27" s="1">
         <v>2008</v>
       </c>
-      <c r="E27" s="10" t="s">
+      <c r="E27" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="F27" s="10"/>
-      <c r="G27" s="10"/>
-      <c r="H27" s="10"/>
-      <c r="I27" s="10"/>
-      <c r="J27" s="10"/>
-      <c r="K27" s="10"/>
-      <c r="L27" s="10"/>
+      <c r="F27" s="11"/>
+      <c r="G27" s="11"/>
+      <c r="H27" s="11"/>
+      <c r="I27" s="11"/>
+      <c r="J27" s="11"/>
+      <c r="K27" s="11"/>
+      <c r="L27" s="11"/>
       <c r="M27" s="6" t="s">
         <v>37</v>
       </c>
@@ -1495,16 +1543,16 @@
       <c r="D28" s="1">
         <v>2015</v>
       </c>
-      <c r="E28" s="10" t="s">
+      <c r="E28" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="F28" s="10"/>
-      <c r="G28" s="10"/>
-      <c r="H28" s="10"/>
-      <c r="I28" s="10"/>
-      <c r="J28" s="10"/>
-      <c r="K28" s="10"/>
-      <c r="L28" s="10"/>
+      <c r="F28" s="11"/>
+      <c r="G28" s="11"/>
+      <c r="H28" s="11"/>
+      <c r="I28" s="11"/>
+      <c r="J28" s="11"/>
+      <c r="K28" s="11"/>
+      <c r="L28" s="11"/>
       <c r="M28" s="6" t="s">
         <v>37</v>
       </c>
@@ -1525,16 +1573,16 @@
       <c r="D29" s="1">
         <v>2016</v>
       </c>
-      <c r="E29" s="10" t="s">
+      <c r="E29" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="F29" s="10"/>
-      <c r="G29" s="10"/>
-      <c r="H29" s="10"/>
-      <c r="I29" s="10"/>
-      <c r="J29" s="10"/>
-      <c r="K29" s="10"/>
-      <c r="L29" s="10"/>
+      <c r="F29" s="11"/>
+      <c r="G29" s="11"/>
+      <c r="H29" s="11"/>
+      <c r="I29" s="11"/>
+      <c r="J29" s="11"/>
+      <c r="K29" s="11"/>
+      <c r="L29" s="11"/>
       <c r="M29" s="6" t="s">
         <v>37</v>
       </c>
@@ -1555,16 +1603,16 @@
       <c r="D30" s="1">
         <v>1996</v>
       </c>
-      <c r="E30" s="10" t="s">
+      <c r="E30" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="F30" s="10"/>
-      <c r="G30" s="10"/>
-      <c r="H30" s="10"/>
-      <c r="I30" s="10"/>
-      <c r="J30" s="10"/>
-      <c r="K30" s="10"/>
-      <c r="L30" s="10"/>
+      <c r="F30" s="11"/>
+      <c r="G30" s="11"/>
+      <c r="H30" s="11"/>
+      <c r="I30" s="11"/>
+      <c r="J30" s="11"/>
+      <c r="K30" s="11"/>
+      <c r="L30" s="11"/>
       <c r="M30" s="6" t="s">
         <v>37</v>
       </c>
@@ -1585,16 +1633,16 @@
       <c r="D31" s="1">
         <v>1993</v>
       </c>
-      <c r="E31" s="10" t="s">
+      <c r="E31" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="F31" s="10"/>
-      <c r="G31" s="10"/>
-      <c r="H31" s="10"/>
-      <c r="I31" s="10"/>
-      <c r="J31" s="10"/>
-      <c r="K31" s="10"/>
-      <c r="L31" s="10"/>
+      <c r="F31" s="11"/>
+      <c r="G31" s="11"/>
+      <c r="H31" s="11"/>
+      <c r="I31" s="11"/>
+      <c r="J31" s="11"/>
+      <c r="K31" s="11"/>
+      <c r="L31" s="11"/>
       <c r="M31" s="5" t="s">
         <v>37</v>
       </c>
@@ -1620,16 +1668,16 @@
       <c r="D33" s="1">
         <v>2009</v>
       </c>
-      <c r="E33" s="10" t="s">
+      <c r="E33" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="F33" s="10"/>
-      <c r="G33" s="10"/>
-      <c r="H33" s="10"/>
-      <c r="I33" s="10"/>
-      <c r="J33" s="10"/>
-      <c r="K33" s="10"/>
-      <c r="L33" s="10"/>
+      <c r="F33" s="11"/>
+      <c r="G33" s="11"/>
+      <c r="H33" s="11"/>
+      <c r="I33" s="11"/>
+      <c r="J33" s="11"/>
+      <c r="K33" s="11"/>
+      <c r="L33" s="11"/>
       <c r="M33" s="6" t="s">
         <v>37</v>
       </c>
@@ -1650,16 +1698,16 @@
       <c r="D34" s="1">
         <v>2013</v>
       </c>
-      <c r="E34" s="10" t="s">
+      <c r="E34" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="F34" s="10"/>
-      <c r="G34" s="10"/>
-      <c r="H34" s="10"/>
-      <c r="I34" s="10"/>
-      <c r="J34" s="10"/>
-      <c r="K34" s="10"/>
-      <c r="L34" s="10"/>
+      <c r="F34" s="11"/>
+      <c r="G34" s="11"/>
+      <c r="H34" s="11"/>
+      <c r="I34" s="11"/>
+      <c r="J34" s="11"/>
+      <c r="K34" s="11"/>
+      <c r="L34" s="11"/>
       <c r="M34" s="9" t="s">
         <v>91</v>
       </c>
@@ -1677,22 +1725,207 @@
       <c r="D35" s="1">
         <v>2005</v>
       </c>
-      <c r="E35" s="10" t="s">
+      <c r="E35" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="F35" s="10"/>
-      <c r="G35" s="10"/>
-      <c r="H35" s="10"/>
-      <c r="I35" s="10"/>
-      <c r="J35" s="10"/>
-      <c r="K35" s="10"/>
-      <c r="L35" s="10"/>
+      <c r="F35" s="11"/>
+      <c r="G35" s="11"/>
+      <c r="H35" s="11"/>
+      <c r="I35" s="11"/>
+      <c r="J35" s="11"/>
+      <c r="K35" s="11"/>
+      <c r="L35" s="11"/>
       <c r="M35" s="9" t="s">
         <v>37</v>
       </c>
     </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A36" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E36" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="F36" s="11"/>
+      <c r="G36" s="11"/>
+      <c r="H36" s="11"/>
+      <c r="I36" s="11"/>
+      <c r="J36" s="11"/>
+      <c r="K36" s="11"/>
+      <c r="L36" s="11"/>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A37" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D37" s="15">
+        <v>42897</v>
+      </c>
+      <c r="E37" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="F37" s="11"/>
+      <c r="G37" s="11"/>
+      <c r="H37" s="11"/>
+      <c r="I37" s="11"/>
+      <c r="J37" s="11"/>
+      <c r="K37" s="11"/>
+      <c r="L37" s="11"/>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A38" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D38" s="15">
+        <v>42532</v>
+      </c>
+      <c r="E38" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="F38" s="11"/>
+      <c r="G38" s="11"/>
+      <c r="H38" s="11"/>
+      <c r="I38" s="11"/>
+      <c r="J38" s="11"/>
+      <c r="K38" s="11"/>
+      <c r="L38" s="11"/>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A39" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D39" s="1">
+        <v>2008</v>
+      </c>
+      <c r="E39" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="F39" s="11"/>
+      <c r="G39" s="11"/>
+      <c r="H39" s="11"/>
+      <c r="I39" s="11"/>
+      <c r="J39" s="11"/>
+      <c r="K39" s="11"/>
+      <c r="L39" s="11"/>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A40" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D40" s="1">
+        <v>2009</v>
+      </c>
+      <c r="E40" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="F40" s="11"/>
+      <c r="G40" s="11"/>
+      <c r="H40" s="11"/>
+      <c r="I40" s="11"/>
+      <c r="J40" s="11"/>
+      <c r="K40" s="11"/>
+      <c r="L40" s="11"/>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A41" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E41" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="F41" s="11"/>
+      <c r="G41" s="11"/>
+      <c r="H41" s="11"/>
+      <c r="I41" s="11"/>
+      <c r="J41" s="11"/>
+      <c r="K41" s="11"/>
+      <c r="L41" s="11"/>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A42" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E42" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="F42" s="11"/>
+      <c r="G42" s="11"/>
+      <c r="H42" s="11"/>
+      <c r="I42" s="11"/>
+      <c r="J42" s="11"/>
+      <c r="K42" s="11"/>
+      <c r="L42" s="11"/>
+    </row>
   </sheetData>
-  <mergeCells count="33">
+  <mergeCells count="40">
+    <mergeCell ref="E14:L14"/>
+    <mergeCell ref="E15:L15"/>
+    <mergeCell ref="E42:L42"/>
+    <mergeCell ref="E41:L41"/>
+    <mergeCell ref="E40:L40"/>
+    <mergeCell ref="E39:L39"/>
+    <mergeCell ref="E38:L38"/>
+    <mergeCell ref="E37:L37"/>
+    <mergeCell ref="E36:L36"/>
+    <mergeCell ref="E13:L13"/>
+    <mergeCell ref="A2:M2"/>
+    <mergeCell ref="E3:L3"/>
+    <mergeCell ref="E4:L4"/>
+    <mergeCell ref="E5:L5"/>
+    <mergeCell ref="E6:L6"/>
+    <mergeCell ref="E7:L7"/>
+    <mergeCell ref="E8:L8"/>
+    <mergeCell ref="E9:L9"/>
+    <mergeCell ref="E10:L10"/>
+    <mergeCell ref="E11:L11"/>
+    <mergeCell ref="E12:L12"/>
+    <mergeCell ref="E16:L16"/>
+    <mergeCell ref="E17:L17"/>
+    <mergeCell ref="E18:L18"/>
+    <mergeCell ref="E19:L19"/>
+    <mergeCell ref="E20:L20"/>
     <mergeCell ref="E35:L35"/>
     <mergeCell ref="E21:L21"/>
     <mergeCell ref="E22:L22"/>
@@ -1705,27 +1938,8 @@
     <mergeCell ref="E30:L30"/>
     <mergeCell ref="E28:L28"/>
     <mergeCell ref="E31:L31"/>
-    <mergeCell ref="E16:L16"/>
-    <mergeCell ref="E17:L17"/>
-    <mergeCell ref="E18:L18"/>
-    <mergeCell ref="E19:L19"/>
-    <mergeCell ref="E20:L20"/>
     <mergeCell ref="E34:L34"/>
-    <mergeCell ref="E13:L13"/>
-    <mergeCell ref="A2:M2"/>
-    <mergeCell ref="E3:L3"/>
-    <mergeCell ref="E4:L4"/>
-    <mergeCell ref="E5:L5"/>
-    <mergeCell ref="E6:L6"/>
-    <mergeCell ref="E7:L7"/>
-    <mergeCell ref="E8:L8"/>
-    <mergeCell ref="E9:L9"/>
-    <mergeCell ref="E10:L10"/>
-    <mergeCell ref="E11:L11"/>
-    <mergeCell ref="E12:L12"/>
     <mergeCell ref="E25:L25"/>
-    <mergeCell ref="E14:L14"/>
-    <mergeCell ref="E15:L15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>